<commit_message>
Update rkkp requested variables from Omar
</commit_message>
<xml_diff>
--- a/data-raw/rkkp/2023-02-03_Variabeloversigt_DIABASE.xlsx
+++ b/data-raw/rkkp/2023-02-03_Variabeloversigt_DIABASE.xlsx
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,7 +989,7 @@
     </row>
     <row r="17" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>11</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="27" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
protocol for rkkp, plus respåond to requests
</commit_message>
<xml_diff>
--- a/data-raw/rkkp/2023-02-03_Variabeloversigt_DIABASE.xlsx
+++ b/data-raw/rkkp/2023-02-03_Variabeloversigt_DIABASE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="102">
   <si>
     <t xml:space="preserve">Variabeloversigt for  Landsdækkende klinisk kvalitetsdatabase for screening af diabetisk retinopati og maculopati</t>
   </si>
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -988,9 +988,7 @@
       <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="A17" s="6"/>
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>

</xml_diff>